<commit_message>
add Login Form add Dashboard for General User with page turner (20コンテンツ、3ページ) edit Menu Bar : Menu 1 -> 4 : sub Menu None, Menu 5,6 : submenu added
</commit_message>
<xml_diff>
--- a/DOC/AWS環境におけるWeb-Blog構築.xlsx
+++ b/DOC/AWS環境におけるWeb-Blog構築.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\目標設定\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebBlog\RepoGitlab\blogweb\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DE5BA4-8EC2-47CE-909C-B1D53F0002D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89BE0BD-197C-4330-B12E-BE02DA4772F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CF7611B0-CE80-435D-9DE3-E718E7AF680B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CF7611B0-CE80-435D-9DE3-E718E7AF680B}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -1499,7 +1499,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1603,9 +1603,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3272,6 +3269,151 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>コンテンツを新規作成</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Speech Bubble: Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C631E71-A753-1B26-8ED0-E2AEE757A8D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9311640" y="3558540"/>
+          <a:ext cx="3581400" cy="2484120"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -23173"/>
+            <a:gd name="adj2" fmla="val 86701"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ダッシュボード：一般ユーザーモードのみ</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>管理者モード、ダッシュボード　→</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>tạo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> 1 màn hình mới,màn hình AD, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>bên trái  có nút tạo mới, hiển thị danh sách bài log </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>bên</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> dưới mỗi bài log sẽ thêm 2 nút nhấn là edit và delete</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>hiển thị đầu tiên là theo từng menu-chủ đề , mỗi chủ đề sẽ có 3 bài viết mới nhất</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>cấu hình cho nhiều thiết bị , máy tính điện thoại ipad...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>@media css cho từng giao diện</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3794,6 +3936,74 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Speech Bubble: Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF4E015E-245D-49CC-1BE7-8A8EB97E0BF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2209800" y="457200"/>
+          <a:ext cx="1897380" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>thêm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> ngày </a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4396,6 +4606,77 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>本文に絵文字を追加</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Speech Bubble: Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC533C0F-7A63-53D4-B304-B49F0D6F192B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2186940" y="2499360"/>
+          <a:ext cx="2308860" cy="777240"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>thêm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> chức năng add ảnh đại diện cho content</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5412,7 +5693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F9F0C4-DE65-4A95-8DD1-C03F9B05C28A}">
   <dimension ref="B2:AF111"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6328125" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -6101,25 +6384,9 @@
       <c r="C62" s="17"/>
       <c r="I62" s="18"/>
       <c r="J62" s="17"/>
-      <c r="K62" s="35" t="s">
+      <c r="K62" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
-      <c r="O62" s="35"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="35"/>
-      <c r="S62" s="35"/>
-      <c r="T62" s="35"/>
-      <c r="U62" s="35"/>
-      <c r="V62" s="35"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
-      <c r="Y62" s="35"/>
-      <c r="Z62" s="35"/>
-      <c r="AA62" s="35"/>
       <c r="AB62" s="18"/>
     </row>
     <row r="63" spans="2:32" x14ac:dyDescent="0.5">
@@ -6127,25 +6394,9 @@
       <c r="C63" s="17"/>
       <c r="I63" s="18"/>
       <c r="J63" s="17"/>
-      <c r="K63" s="35" t="s">
+      <c r="K63" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
-      <c r="O63" s="35"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="35"/>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35"/>
-      <c r="T63" s="35"/>
-      <c r="U63" s="35"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
-      <c r="Z63" s="35"/>
-      <c r="AA63" s="35"/>
       <c r="AB63" s="18"/>
     </row>
     <row r="64" spans="2:32" x14ac:dyDescent="0.5">
@@ -6155,23 +6406,6 @@
       <c r="J64" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="K64" s="35"/>
-      <c r="L64" s="35"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="35"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="35"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="35"/>
-      <c r="S64" s="35"/>
-      <c r="T64" s="35"/>
-      <c r="U64" s="35"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
-      <c r="Z64" s="35"/>
-      <c r="AA64" s="35"/>
       <c r="AB64" s="18"/>
     </row>
     <row r="65" spans="2:28" x14ac:dyDescent="0.5">
@@ -6179,87 +6413,29 @@
       <c r="C65" s="17"/>
       <c r="I65" s="18"/>
       <c r="J65" s="17"/>
-      <c r="K65" s="35" t="s">
+      <c r="K65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="35"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="35"/>
-      <c r="R65" s="35"/>
-      <c r="S65" s="35"/>
-      <c r="T65" s="35"/>
-      <c r="U65" s="35"/>
-      <c r="V65" s="35"/>
-      <c r="W65" s="35"/>
-      <c r="X65" s="35"/>
-      <c r="Y65" s="35"/>
-      <c r="Z65" s="35"/>
-      <c r="AA65" s="35"/>
       <c r="AB65" s="18"/>
     </row>
     <row r="66" spans="2:28" x14ac:dyDescent="0.5">
       <c r="B66" s="2"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
       <c r="I66" s="18"/>
       <c r="J66" s="17"/>
-      <c r="K66" s="35" t="s">
+      <c r="K66" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="L66" s="35"/>
-      <c r="M66" s="35"/>
-      <c r="N66" s="35"/>
-      <c r="O66" s="35"/>
-      <c r="P66" s="35"/>
-      <c r="Q66" s="35"/>
-      <c r="R66" s="35"/>
-      <c r="S66" s="35"/>
-      <c r="T66" s="35"/>
-      <c r="U66" s="35"/>
-      <c r="V66" s="35"/>
-      <c r="W66" s="35"/>
-      <c r="X66" s="35"/>
-      <c r="Y66" s="35"/>
-      <c r="Z66" s="35"/>
-      <c r="AA66" s="35"/>
       <c r="AB66" s="18"/>
     </row>
     <row r="67" spans="2:28" x14ac:dyDescent="0.5">
       <c r="B67" s="2"/>
       <c r="C67" s="17"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
       <c r="I67" s="18"/>
       <c r="J67" s="17"/>
-      <c r="K67" s="35" t="s">
+      <c r="K67" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="L67" s="35"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="35"/>
-      <c r="O67" s="35"/>
-      <c r="P67" s="35"/>
-      <c r="Q67" s="35"/>
-      <c r="R67" s="35"/>
-      <c r="S67" s="35"/>
-      <c r="T67" s="35"/>
-      <c r="U67" s="35"/>
-      <c r="V67" s="35"/>
-      <c r="W67" s="35"/>
-      <c r="X67" s="35"/>
-      <c r="Y67" s="35"/>
-      <c r="Z67" s="35"/>
-      <c r="AA67" s="35"/>
       <c r="AB67" s="18"/>
     </row>
     <row r="68" spans="2:28" x14ac:dyDescent="0.5">
@@ -6327,182 +6503,56 @@
       <c r="C70" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="35"/>
       <c r="I70" s="18"/>
       <c r="J70" s="17"/>
-      <c r="K70" s="35" t="s">
+      <c r="K70" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="L70" s="35"/>
-      <c r="M70" s="35"/>
-      <c r="N70" s="35"/>
-      <c r="O70" s="35"/>
-      <c r="P70" s="35"/>
-      <c r="Q70" s="35"/>
-      <c r="R70" s="35"/>
-      <c r="S70" s="35"/>
-      <c r="T70" s="35"/>
-      <c r="U70" s="35"/>
-      <c r="V70" s="35"/>
-      <c r="W70" s="35"/>
-      <c r="X70" s="35"/>
-      <c r="Y70" s="35"/>
-      <c r="Z70" s="35"/>
-      <c r="AA70" s="35"/>
       <c r="AB70" s="18"/>
     </row>
     <row r="71" spans="2:28" x14ac:dyDescent="0.5">
       <c r="C71" s="17"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
       <c r="I71" s="18"/>
       <c r="J71" s="17"/>
-      <c r="K71" s="35"/>
-      <c r="L71" s="35" t="s">
+      <c r="L71" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="M71" s="35"/>
-      <c r="N71" s="35"/>
-      <c r="O71" s="35"/>
-      <c r="P71" s="35"/>
-      <c r="Q71" s="35"/>
-      <c r="R71" s="35"/>
-      <c r="S71" s="35"/>
-      <c r="T71" s="35"/>
-      <c r="U71" s="35"/>
-      <c r="V71" s="35"/>
-      <c r="W71" s="35"/>
-      <c r="X71" s="35"/>
-      <c r="Y71" s="35"/>
-      <c r="Z71" s="35"/>
-      <c r="AA71" s="35"/>
       <c r="AB71" s="18"/>
     </row>
     <row r="72" spans="2:28" x14ac:dyDescent="0.5">
       <c r="C72" s="17"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="35"/>
       <c r="I72" s="18"/>
       <c r="J72" s="17"/>
-      <c r="K72" s="35"/>
-      <c r="L72" s="35" t="s">
+      <c r="L72" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="M72" s="35"/>
-      <c r="N72" s="35"/>
-      <c r="O72" s="35"/>
-      <c r="P72" s="35"/>
-      <c r="Q72" s="35"/>
-      <c r="R72" s="35"/>
-      <c r="S72" s="35"/>
-      <c r="T72" s="35"/>
-      <c r="U72" s="35"/>
-      <c r="V72" s="35"/>
-      <c r="W72" s="35"/>
-      <c r="X72" s="35"/>
-      <c r="Y72" s="35"/>
-      <c r="Z72" s="35"/>
-      <c r="AA72" s="35"/>
       <c r="AB72" s="18"/>
     </row>
     <row r="73" spans="2:28" x14ac:dyDescent="0.5">
       <c r="C73" s="17"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="35"/>
       <c r="I73" s="18"/>
       <c r="J73" s="17"/>
-      <c r="K73" s="35"/>
-      <c r="L73" s="35"/>
-      <c r="M73" s="35"/>
-      <c r="N73" s="35"/>
-      <c r="O73" s="35"/>
-      <c r="P73" s="35"/>
-      <c r="Q73" s="35"/>
-      <c r="R73" s="35"/>
-      <c r="S73" s="35"/>
-      <c r="T73" s="35"/>
-      <c r="U73" s="35"/>
-      <c r="V73" s="35"/>
-      <c r="W73" s="35"/>
-      <c r="X73" s="35"/>
-      <c r="Y73" s="35"/>
-      <c r="Z73" s="35"/>
-      <c r="AA73" s="35"/>
       <c r="AB73" s="18"/>
     </row>
     <row r="74" spans="2:28" x14ac:dyDescent="0.5">
       <c r="C74" s="17"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="35"/>
       <c r="I74" s="18"/>
       <c r="J74" s="17"/>
-      <c r="K74" s="35" t="s">
+      <c r="K74" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="L74" s="35"/>
-      <c r="M74" s="35"/>
-      <c r="N74" s="35"/>
-      <c r="O74" s="35"/>
-      <c r="P74" s="35"/>
-      <c r="Q74" s="35"/>
-      <c r="R74" s="35"/>
-      <c r="S74" s="35"/>
-      <c r="T74" s="35"/>
-      <c r="U74" s="35"/>
-      <c r="V74" s="35"/>
-      <c r="W74" s="35"/>
-      <c r="X74" s="35"/>
-      <c r="Y74" s="35"/>
-      <c r="Z74" s="35"/>
-      <c r="AA74" s="35"/>
       <c r="AB74" s="18"/>
     </row>
     <row r="75" spans="2:28" x14ac:dyDescent="0.5">
       <c r="C75" s="17"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
       <c r="I75" s="18"/>
       <c r="J75" s="17"/>
-      <c r="K75" s="35" t="s">
+      <c r="K75" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L75" s="35" t="s">
+      <c r="L75" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="M75" s="35"/>
-      <c r="N75" s="35"/>
-      <c r="O75" s="35"/>
-      <c r="P75" s="35"/>
-      <c r="Q75" s="35"/>
-      <c r="R75" s="35"/>
-      <c r="S75" s="35"/>
-      <c r="T75" s="35"/>
-      <c r="U75" s="35"/>
-      <c r="V75" s="35"/>
-      <c r="W75" s="35"/>
-      <c r="X75" s="35"/>
-      <c r="Y75" s="35"/>
-      <c r="Z75" s="35"/>
-      <c r="AA75" s="35"/>
       <c r="AB75" s="18"/>
     </row>
     <row r="76" spans="2:28" x14ac:dyDescent="0.5">
@@ -6747,23 +6797,6 @@
       <c r="J84" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K84" s="35"/>
-      <c r="L84" s="35"/>
-      <c r="M84" s="35"/>
-      <c r="N84" s="35"/>
-      <c r="O84" s="35"/>
-      <c r="P84" s="35"/>
-      <c r="Q84" s="35"/>
-      <c r="R84" s="35"/>
-      <c r="S84" s="35"/>
-      <c r="T84" s="35"/>
-      <c r="U84" s="35"/>
-      <c r="V84" s="35"/>
-      <c r="W84" s="35"/>
-      <c r="X84" s="35"/>
-      <c r="Y84" s="35"/>
-      <c r="Z84" s="35"/>
-      <c r="AA84" s="35"/>
       <c r="AB84" s="18"/>
     </row>
     <row r="85" spans="3:28" x14ac:dyDescent="0.5">
@@ -6775,23 +6808,6 @@
       <c r="J85" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="K85" s="35"/>
-      <c r="L85" s="35"/>
-      <c r="M85" s="35"/>
-      <c r="N85" s="35"/>
-      <c r="O85" s="35"/>
-      <c r="P85" s="35"/>
-      <c r="Q85" s="35"/>
-      <c r="R85" s="35"/>
-      <c r="S85" s="35"/>
-      <c r="T85" s="35"/>
-      <c r="U85" s="35"/>
-      <c r="V85" s="35"/>
-      <c r="W85" s="35"/>
-      <c r="X85" s="35"/>
-      <c r="Y85" s="35"/>
-      <c r="Z85" s="35"/>
-      <c r="AA85" s="35"/>
       <c r="AB85" s="18"/>
     </row>
     <row r="86" spans="3:28" x14ac:dyDescent="0.5">
@@ -6868,7 +6884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72953D3A-CB52-4553-B532-CBD34C1DAB0D}">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6328125" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -6892,7 +6910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACB3C75-F876-4AB2-AF03-2BE046DA6FCD}">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6328125" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>

</xml_diff>